<commit_message>
begin to developed the admin panel.
</commit_message>
<xml_diff>
--- a/Calibration/Reports/USBCWood.xlsx
+++ b/Calibration/Reports/USBCWood.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="105" yWindow="105" windowWidth="9000" windowHeight="7995"/>
+    <workbookView xWindow="105" yWindow="105" windowWidth="9000" windowHeight="7995" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="USBC Report (1-16)" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="109">
   <si>
     <t>Certification #</t>
   </si>
@@ -174,9 +174,6 @@
     <t>Distance</t>
   </si>
   <si>
-    <t>Middle Of Lane</t>
-  </si>
-  <si>
     <t>Measure Between     30'-40'</t>
   </si>
   <si>
@@ -403,30 +400,6 @@
   </si>
   <si>
     <t>Description</t>
-  </si>
-  <si>
-    <t>Cross</t>
-  </si>
-  <si>
-    <t>Length</t>
-  </si>
-  <si>
-    <t>6 to 12 7Side</t>
-  </si>
-  <si>
-    <t>6 to 12 10 Side</t>
-  </si>
-  <si>
-    <t>9 to 15 7 side</t>
-  </si>
-  <si>
-    <t>9 to 15 10 side</t>
-  </si>
-  <si>
-    <t>12 to 18 7 Side</t>
-  </si>
-  <si>
-    <t>12 to 18 10 Side</t>
   </si>
   <si>
     <t>Right 10 board</t>
@@ -442,7 +415,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -1015,6 +988,42 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1074,42 +1083,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1440,11 +1413,11 @@
   <sheetPr codeName="USBC Report (1-16)"/>
   <dimension ref="A3:V34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="70" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
@@ -1454,55 +1427,55 @@
     <col min="7" max="22" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:22" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C3" s="51" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
+    <row r="3" spans="1:22" s="1" customFormat="1" ht="27" customHeight="1">
+      <c r="C3" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
       <c r="F3" s="3" t="str">
         <f>LaneData!B5</f>
         <v>300</v>
       </c>
-      <c r="H3" s="52" t="s">
+      <c r="H3" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="50" t="str">
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="28" t="str">
         <f>LaneData!B3</f>
         <v>USBC_Data_1-4_O</v>
       </c>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50"/>
-      <c r="Q3" s="50"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
+      <c r="Q3" s="28"/>
       <c r="S3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="T3" s="49" t="str">
+      <c r="T3" s="27" t="str">
         <f>LaneData!B4</f>
         <v>2/2/2012</v>
       </c>
-      <c r="U3" s="49"/>
-    </row>
-    <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="U3" s="27"/>
+    </row>
+    <row r="4" spans="1:22" ht="15" customHeight="1"/>
+    <row r="5" spans="1:22" ht="18.75" customHeight="1">
       <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" ht="18.75" customHeight="1">
       <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" ht="18.75" customHeight="1">
       <c r="A7" s="4"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22">
       <c r="G8" s="5" t="s">
         <v>5</v>
       </c>
@@ -1552,17 +1525,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" ht="40.5" customHeight="1">
       <c r="A9" s="6"/>
-      <c r="B9" s="58" t="s">
+      <c r="B9" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="54"/>
-      <c r="D9" s="55" t="s">
+      <c r="C9" s="32"/>
+      <c r="D9" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
       <c r="G9" s="7" t="str">
         <f>LaneData!C7</f>
         <v>L1</v>
@@ -1628,38 +1601,38 @@
         <v>L16</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
-      <c r="B10" s="28" t="s">
+    <row r="10" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A10" s="39"/>
+      <c r="B10" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="29"/>
-      <c r="D10" s="30" t="s">
+      <c r="C10" s="41"/>
+      <c r="D10" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="32" t="s">
+      <c r="E10" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="33"/>
+      <c r="F10" s="45"/>
       <c r="G10" s="8">
         <f>LaneData!C8</f>
-        <v>-11</v>
+        <v>0</v>
       </c>
       <c r="H10" s="8">
         <f>LaneData!D8</f>
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="I10" s="8">
         <f>LaneData!E8</f>
-        <v>-12</v>
+        <v>0</v>
       </c>
       <c r="J10" s="8">
         <f>LaneData!F8</f>
-        <v>-11</v>
+        <v>0</v>
       </c>
       <c r="K10" s="8">
         <f>LaneData!G8</f>
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="L10" s="8">
         <f>LaneData!H8</f>
@@ -1706,37 +1679,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="27"/>
-      <c r="B11" s="34">
+    <row r="11" spans="1:22" ht="40.5" customHeight="1" thickBot="1">
+      <c r="A11" s="39"/>
+      <c r="B11" s="46">
         <f>LaneData!A8</f>
-        <v>15</v>
-      </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="47"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="38"/>
+      <c r="F11" s="50"/>
       <c r="G11" s="8">
         <f>LaneData!C9</f>
-        <v>-56</v>
+        <v>0</v>
       </c>
       <c r="H11" s="8">
         <f>LaneData!D9</f>
-        <v>-54</v>
+        <v>0</v>
       </c>
       <c r="I11" s="8">
         <f>LaneData!E9</f>
-        <v>-57</v>
+        <v>0</v>
       </c>
       <c r="J11" s="8">
         <f>LaneData!F9</f>
-        <v>-51</v>
+        <v>0</v>
       </c>
       <c r="K11" s="8">
         <f>LaneData!G9</f>
-        <v>-55</v>
+        <v>0</v>
       </c>
       <c r="L11" s="8">
         <f>LaneData!H9</f>
@@ -1783,36 +1756,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="27"/>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="39" t="s">
+    <row r="12" spans="1:22" ht="40.5" customHeight="1" thickBot="1">
+      <c r="A12" s="39"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="42" t="s">
-        <v>115</v>
-      </c>
-      <c r="F12" s="33"/>
+      <c r="E12" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="F12" s="45"/>
       <c r="G12" s="8">
         <f>LaneData!C10</f>
-        <v>-7</v>
+        <v>0</v>
       </c>
       <c r="H12" s="8">
         <f>LaneData!D10</f>
-        <v>-7</v>
+        <v>0</v>
       </c>
       <c r="I12" s="8">
         <f>LaneData!E10</f>
-        <v>-7</v>
+        <v>0</v>
       </c>
       <c r="J12" s="8">
         <f>LaneData!F10</f>
-        <v>-7</v>
+        <v>0</v>
       </c>
       <c r="K12" s="8">
         <f>LaneData!G10</f>
-        <v>-7</v>
+        <v>0</v>
       </c>
       <c r="L12" s="8">
         <f>LaneData!H10</f>
@@ -1859,36 +1832,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
-      <c r="B13" s="43" t="s">
+    <row r="13" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A13" s="39"/>
+      <c r="B13" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="44"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="45" t="s">
-        <v>116</v>
-      </c>
-      <c r="F13" s="46"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="57" t="s">
+        <v>107</v>
+      </c>
+      <c r="F13" s="58"/>
       <c r="G13" s="8">
         <f>LaneData!C11</f>
-        <v>-18</v>
+        <v>0</v>
       </c>
       <c r="H13" s="8">
         <f>LaneData!D11</f>
-        <v>-18</v>
+        <v>0</v>
       </c>
       <c r="I13" s="8">
         <f>LaneData!E11</f>
-        <v>-18</v>
+        <v>0</v>
       </c>
       <c r="J13" s="8">
         <f>LaneData!F11</f>
-        <v>-18</v>
+        <v>0</v>
       </c>
       <c r="K13" s="8">
         <f>LaneData!G11</f>
-        <v>-18</v>
+        <v>0</v>
       </c>
       <c r="L13" s="8">
         <f>LaneData!H11</f>
@@ -1935,34 +1908,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" ht="40.5" customHeight="1" thickBot="1">
       <c r="A14" s="9"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="47" t="s">
-        <v>117</v>
-      </c>
-      <c r="F14" s="48"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="F14" s="38"/>
       <c r="G14" s="8">
         <f>LaneData!C12</f>
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H14" s="8">
         <f>LaneData!D12</f>
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="I14" s="8">
         <f>LaneData!E12</f>
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="J14" s="8">
         <f>LaneData!F12</f>
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="K14" s="8">
         <f>LaneData!G12</f>
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="L14" s="8">
         <f>LaneData!H12</f>
@@ -2009,7 +1982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22">
       <c r="A15" s="11"/>
       <c r="B15" s="12"/>
       <c r="G15" s="5" t="s">
@@ -2061,17 +2034,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" ht="40.5" customHeight="1">
       <c r="A16" s="6"/>
-      <c r="B16" s="56" t="s">
+      <c r="B16" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="57"/>
-      <c r="D16" s="55" t="s">
+      <c r="C16" s="35"/>
+      <c r="D16" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
       <c r="G16" s="7" t="str">
         <f>LaneData!C7</f>
         <v>L1</v>
@@ -2137,38 +2110,38 @@
         <v>L16</v>
       </c>
     </row>
-    <row r="17" spans="1:22" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="27"/>
-      <c r="B17" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="29"/>
-      <c r="D17" s="30" t="s">
+    <row r="17" spans="1:22" ht="40.5" customHeight="1" thickBot="1">
+      <c r="A17" s="39"/>
+      <c r="B17" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="41"/>
+      <c r="D17" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="32" t="s">
+      <c r="E17" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="33"/>
+      <c r="F17" s="45"/>
       <c r="G17" s="8">
         <f>LaneData!C13</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H17" s="8">
         <f>LaneData!D13</f>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="I17" s="8">
         <f>LaneData!E13</f>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="J17" s="8">
         <f>LaneData!F13</f>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="K17" s="8">
         <f>LaneData!G13</f>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="L17" s="8">
         <f>LaneData!H13</f>
@@ -2215,37 +2188,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="27"/>
-      <c r="B18" s="34">
+    <row r="18" spans="1:22" ht="40.5" customHeight="1" thickBot="1">
+      <c r="A18" s="39"/>
+      <c r="B18" s="46">
         <f>LaneData!A13</f>
-        <v>30</v>
-      </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="47"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="38"/>
+      <c r="F18" s="50"/>
       <c r="G18" s="8">
         <f>LaneData!C14</f>
-        <v>-166</v>
+        <v>0</v>
       </c>
       <c r="H18" s="8">
         <f>LaneData!D14</f>
-        <v>-171</v>
+        <v>0</v>
       </c>
       <c r="I18" s="8">
         <f>LaneData!E14</f>
-        <v>-169</v>
+        <v>0</v>
       </c>
       <c r="J18" s="8">
         <f>LaneData!F14</f>
-        <v>-172</v>
+        <v>0</v>
       </c>
       <c r="K18" s="8">
         <f>LaneData!G14</f>
-        <v>-167</v>
+        <v>0</v>
       </c>
       <c r="L18" s="8">
         <f>LaneData!H14</f>
@@ -2292,17 +2265,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="27"/>
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="39" t="s">
+    <row r="19" spans="1:22" ht="40.5" customHeight="1" thickBot="1">
+      <c r="A19" s="39"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="42" t="s">
-        <v>115</v>
-      </c>
-      <c r="F19" s="33"/>
+      <c r="E19" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="F19" s="45"/>
       <c r="G19" s="8">
         <f>LaneData!C15</f>
         <v>0</v>
@@ -2368,36 +2341,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
-      <c r="B20" s="43" t="s">
+    <row r="20" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A20" s="39"/>
+      <c r="B20" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="44"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="45" t="s">
-        <v>116</v>
-      </c>
-      <c r="F20" s="46"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="57" t="s">
+        <v>107</v>
+      </c>
+      <c r="F20" s="58"/>
       <c r="G20" s="8">
         <f>LaneData!C16</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H20" s="8">
         <f>LaneData!D16</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I20" s="8">
         <f>LaneData!E16</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J20" s="8">
         <f>LaneData!F16</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K20" s="8">
         <f>LaneData!G16</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L20" s="8">
         <f>LaneData!H16</f>
@@ -2444,34 +2417,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:22" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" ht="40.5" customHeight="1" thickBot="1">
       <c r="A21" s="9"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="47" t="s">
-        <v>117</v>
-      </c>
-      <c r="F21" s="48"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="F21" s="38"/>
       <c r="G21" s="8">
         <f>LaneData!C17</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H21" s="8">
         <f>LaneData!D17</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I21" s="8">
         <f>LaneData!E17</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J21" s="8">
         <f>LaneData!F17</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K21" s="8">
         <f>LaneData!G17</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L21" s="8">
         <f>LaneData!H17</f>
@@ -2518,7 +2491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22">
       <c r="A22" s="11"/>
       <c r="B22" s="13"/>
       <c r="G22" s="5" t="s">
@@ -2570,17 +2543,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" ht="40.5" customHeight="1">
       <c r="A23" s="6"/>
-      <c r="B23" s="53" t="s">
+      <c r="B23" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="54"/>
-      <c r="D23" s="55" t="s">
+      <c r="C23" s="32"/>
+      <c r="D23" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="55"/>
-      <c r="F23" s="55"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="33"/>
       <c r="G23" s="7" t="str">
         <f>LaneData!C7</f>
         <v>L1</v>
@@ -2646,38 +2619,38 @@
         <v>L16</v>
       </c>
     </row>
-    <row r="24" spans="1:22" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="27"/>
-      <c r="B24" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="29"/>
-      <c r="D24" s="30" t="s">
+    <row r="24" spans="1:22" ht="40.5" customHeight="1" thickBot="1">
+      <c r="A24" s="39"/>
+      <c r="B24" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="41"/>
+      <c r="D24" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="32" t="s">
+      <c r="E24" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="F24" s="33"/>
+      <c r="F24" s="45"/>
       <c r="G24" s="8">
         <f>LaneData!C18</f>
-        <v>-15</v>
+        <v>0</v>
       </c>
       <c r="H24" s="8">
         <f>LaneData!D18</f>
-        <v>-9</v>
+        <v>0</v>
       </c>
       <c r="I24" s="8">
         <f>LaneData!E18</f>
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="J24" s="8">
         <f>LaneData!F18</f>
-        <v>-8</v>
+        <v>0</v>
       </c>
       <c r="K24" s="8">
         <f>LaneData!G18</f>
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="L24" s="8">
         <f>LaneData!H18</f>
@@ -2724,37 +2697,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:22" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="27"/>
-      <c r="B25" s="34">
+    <row r="25" spans="1:22" ht="40.5" customHeight="1" thickBot="1">
+      <c r="A25" s="39"/>
+      <c r="B25" s="46">
         <f>LaneData!A18</f>
-        <v>55</v>
-      </c>
-      <c r="C25" s="35"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="47"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="F25" s="38"/>
+      <c r="F25" s="50"/>
       <c r="G25" s="8">
         <f>LaneData!C19</f>
-        <v>-139</v>
+        <v>0</v>
       </c>
       <c r="H25" s="8">
         <f>LaneData!D19</f>
-        <v>-141</v>
+        <v>0</v>
       </c>
       <c r="I25" s="8">
         <f>LaneData!E19</f>
-        <v>-144</v>
+        <v>0</v>
       </c>
       <c r="J25" s="8">
         <f>LaneData!F19</f>
-        <v>-145</v>
+        <v>0</v>
       </c>
       <c r="K25" s="8">
         <f>LaneData!G19</f>
-        <v>-138</v>
+        <v>0</v>
       </c>
       <c r="L25" s="8">
         <f>LaneData!H19</f>
@@ -2801,36 +2774,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:22" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="27"/>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="39" t="s">
+    <row r="26" spans="1:22" ht="40.5" customHeight="1" thickBot="1">
+      <c r="A26" s="39"/>
+      <c r="B26" s="48"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="E26" s="42" t="s">
-        <v>115</v>
-      </c>
-      <c r="F26" s="33"/>
+      <c r="E26" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="F26" s="45"/>
       <c r="G26" s="8">
         <f>LaneData!C20</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H26" s="8">
         <f>LaneData!D20</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I26" s="8">
         <f>LaneData!E20</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J26" s="8">
         <f>LaneData!F20</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K26" s="8">
         <f>LaneData!G20</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L26" s="8">
         <f>LaneData!H20</f>
@@ -2877,36 +2850,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="27"/>
-      <c r="B27" s="43" t="s">
+    <row r="27" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A27" s="39"/>
+      <c r="B27" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="44"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="45" t="s">
-        <v>116</v>
-      </c>
-      <c r="F27" s="46"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="52"/>
+      <c r="E27" s="57" t="s">
+        <v>107</v>
+      </c>
+      <c r="F27" s="58"/>
       <c r="G27" s="8">
         <f>LaneData!C21</f>
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="H27" s="8">
         <f>LaneData!D21</f>
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="I27" s="8">
         <f>LaneData!E21</f>
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="J27" s="8">
         <f>LaneData!F21</f>
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="K27" s="8">
         <f>LaneData!G21</f>
-        <v>-5</v>
+        <v>0</v>
       </c>
       <c r="L27" s="8">
         <f>LaneData!H21</f>
@@ -2953,34 +2926,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:22" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" ht="40.5" customHeight="1" thickBot="1">
       <c r="A28" s="10"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="47" t="s">
-        <v>117</v>
-      </c>
-      <c r="F28" s="48"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="F28" s="38"/>
       <c r="G28" s="8">
         <f>LaneData!C22</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H28" s="8">
         <f>LaneData!D22</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I28" s="8">
         <f>LaneData!E22</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J28" s="8">
         <f>LaneData!F22</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K28" s="8">
         <f>LaneData!G22</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L28" s="8">
         <f>LaneData!H22</f>
@@ -3027,7 +3000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:22" s="11" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" s="11" customFormat="1" ht="10.5" customHeight="1">
       <c r="A29" s="9"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -3051,12 +3024,12 @@
       <c r="U29" s="15"/>
       <c r="V29" s="15"/>
     </row>
-    <row r="30" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:22" ht="21" customHeight="1">
       <c r="A30" s="16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="1:22" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" ht="26.25" customHeight="1">
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
@@ -3080,7 +3053,7 @@
       <c r="U31" s="13"/>
       <c r="V31" s="13"/>
     </row>
-    <row r="32" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" ht="40.5" customHeight="1">
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
       <c r="C32" s="13"/>
@@ -3104,7 +3077,7 @@
       <c r="U32" s="13"/>
       <c r="V32" s="13"/>
     </row>
-    <row r="33" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" ht="40.5" customHeight="1">
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
       <c r="C33" s="13"/>
@@ -3128,21 +3101,33 @@
       <c r="U33" s="13"/>
       <c r="V33" s="13"/>
     </row>
-    <row r="34" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" ht="15.75" customHeight="1">
       <c r="A34" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="L3:Q3"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="B11:C12"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="B18:C19"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
     <mergeCell ref="E28:F28"/>
     <mergeCell ref="A24:A27"/>
     <mergeCell ref="B24:C24"/>
@@ -3154,28 +3139,16 @@
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="E27:F27"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="B18:C19"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="B11:C12"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="L3:Q3"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:F9"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0.5" header="0" footer="0"/>
@@ -3198,7 +3171,7 @@
       <selection activeCell="E26" sqref="E26:F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
@@ -3208,55 +3181,55 @@
     <col min="7" max="22" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:22" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C3" s="51" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
+    <row r="3" spans="1:22" s="1" customFormat="1" ht="27" customHeight="1">
+      <c r="C3" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
       <c r="F3" s="3" t="str">
         <f>LaneData!B5</f>
         <v>300</v>
       </c>
-      <c r="H3" s="52" t="s">
+      <c r="H3" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="50" t="str">
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="28" t="str">
         <f>LaneData!B3</f>
         <v>USBC_Data_1-4_O</v>
       </c>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50"/>
-      <c r="Q3" s="50"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
+      <c r="Q3" s="28"/>
       <c r="S3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="T3" s="49" t="str">
+      <c r="T3" s="27" t="str">
         <f>LaneData!B4</f>
         <v>2/2/2012</v>
       </c>
-      <c r="U3" s="49"/>
-    </row>
-    <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="U3" s="27"/>
+    </row>
+    <row r="4" spans="1:22" ht="15" customHeight="1"/>
+    <row r="5" spans="1:22" ht="18.75" customHeight="1">
       <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" ht="18.75" customHeight="1">
       <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" ht="18.75" customHeight="1">
       <c r="A7" s="4"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22">
       <c r="G8" s="5" t="s">
         <v>5</v>
       </c>
@@ -3306,17 +3279,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" ht="40.5" customHeight="1">
       <c r="A9" s="6"/>
-      <c r="B9" s="58" t="s">
+      <c r="B9" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="54"/>
-      <c r="D9" s="55" t="s">
+      <c r="C9" s="32"/>
+      <c r="D9" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
       <c r="G9" s="7" t="str">
         <f>LaneData!S7</f>
         <v>L17</v>
@@ -3382,19 +3355,19 @@
         <v>L32</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
-      <c r="B10" s="28" t="s">
+    <row r="10" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A10" s="39"/>
+      <c r="B10" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="29"/>
-      <c r="D10" s="30" t="s">
+      <c r="C10" s="41"/>
+      <c r="D10" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="32" t="s">
+      <c r="E10" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="33"/>
+      <c r="F10" s="45"/>
       <c r="G10" s="18">
         <f>LaneData!S8</f>
         <v>0</v>
@@ -3460,18 +3433,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
-      <c r="B11" s="34">
+    <row r="11" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A11" s="39"/>
+      <c r="B11" s="46">
         <f>LaneData!A8</f>
-        <v>15</v>
-      </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="31"/>
+        <v>0</v>
+      </c>
+      <c r="C11" s="47"/>
+      <c r="D11" s="43"/>
       <c r="E11" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="48"/>
+      <c r="F11" s="38"/>
       <c r="G11" s="18">
         <f>LaneData!S9</f>
         <v>0</v>
@@ -3537,17 +3510,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="30" t="s">
+    <row r="12" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A12" s="39"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="42" t="s">
-        <v>115</v>
-      </c>
-      <c r="F12" s="33"/>
+      <c r="E12" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="F12" s="45"/>
       <c r="G12" s="18">
         <f>LaneData!S10</f>
         <v>0</v>
@@ -3613,17 +3586,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
-      <c r="B13" s="43" t="s">
+    <row r="13" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A13" s="39"/>
+      <c r="B13" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="44"/>
+      <c r="C13" s="56"/>
       <c r="D13" s="60"/>
-      <c r="E13" s="45" t="s">
-        <v>116</v>
-      </c>
-      <c r="F13" s="46"/>
+      <c r="E13" s="57" t="s">
+        <v>107</v>
+      </c>
+      <c r="F13" s="58"/>
       <c r="G13" s="18">
         <f>LaneData!S11</f>
         <v>0</v>
@@ -3689,15 +3662,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" ht="40.5" customHeight="1">
       <c r="A14" s="9"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="47" t="s">
-        <v>117</v>
-      </c>
-      <c r="F14" s="48"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="F14" s="38"/>
       <c r="G14" s="18">
         <f>LaneData!S12</f>
         <v>0</v>
@@ -3763,7 +3736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22">
       <c r="A15" s="11"/>
       <c r="B15" s="12"/>
       <c r="G15" s="5" t="s">
@@ -3815,17 +3788,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" ht="40.5" customHeight="1">
       <c r="A16" s="6"/>
-      <c r="B16" s="56" t="s">
+      <c r="B16" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="57"/>
-      <c r="D16" s="55" t="s">
+      <c r="C16" s="35"/>
+      <c r="D16" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
       <c r="G16" s="7" t="str">
         <f>LaneData!S7</f>
         <v>L17</v>
@@ -3891,19 +3864,19 @@
         <v>L32</v>
       </c>
     </row>
-    <row r="17" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
-      <c r="B17" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="29"/>
-      <c r="D17" s="30" t="s">
+    <row r="17" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A17" s="39"/>
+      <c r="B17" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="41"/>
+      <c r="D17" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="32" t="s">
+      <c r="E17" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="33"/>
+      <c r="F17" s="45"/>
       <c r="G17" s="18">
         <f>LaneData!S8</f>
         <v>0</v>
@@ -3969,18 +3942,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
-      <c r="B18" s="34">
+    <row r="18" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A18" s="39"/>
+      <c r="B18" s="46">
         <f>LaneData!A13</f>
-        <v>30</v>
-      </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="31"/>
+        <v>0</v>
+      </c>
+      <c r="C18" s="47"/>
+      <c r="D18" s="43"/>
       <c r="E18" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="48"/>
+      <c r="F18" s="38"/>
       <c r="G18" s="18">
         <f>LaneData!S9</f>
         <v>0</v>
@@ -4046,17 +4019,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="30" t="s">
+    <row r="19" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A19" s="39"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="42" t="s">
-        <v>115</v>
-      </c>
-      <c r="F19" s="33"/>
+      <c r="E19" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="F19" s="45"/>
       <c r="G19" s="18">
         <f>LaneData!S10</f>
         <v>0</v>
@@ -4122,17 +4095,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
-      <c r="B20" s="43" t="s">
+    <row r="20" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A20" s="39"/>
+      <c r="B20" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="44"/>
+      <c r="C20" s="56"/>
       <c r="D20" s="60"/>
-      <c r="E20" s="45" t="s">
-        <v>116</v>
-      </c>
-      <c r="F20" s="46"/>
+      <c r="E20" s="57" t="s">
+        <v>107</v>
+      </c>
+      <c r="F20" s="58"/>
       <c r="G20" s="18">
         <f>LaneData!S11</f>
         <v>0</v>
@@ -4198,15 +4171,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" ht="40.5" customHeight="1">
       <c r="A21" s="9"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="47" t="s">
-        <v>117</v>
-      </c>
-      <c r="F21" s="48"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="F21" s="38"/>
       <c r="G21" s="18">
         <f>LaneData!S12</f>
         <v>0</v>
@@ -4272,7 +4245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22">
       <c r="A22" s="11"/>
       <c r="B22" s="13"/>
       <c r="G22" s="5" t="s">
@@ -4324,17 +4297,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" ht="40.5" customHeight="1">
       <c r="A23" s="6"/>
-      <c r="B23" s="53" t="s">
+      <c r="B23" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="54"/>
-      <c r="D23" s="55" t="s">
+      <c r="C23" s="32"/>
+      <c r="D23" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="55"/>
-      <c r="F23" s="55"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="33"/>
       <c r="G23" s="7" t="str">
         <f>LaneData!S7</f>
         <v>L17</v>
@@ -4400,19 +4373,19 @@
         <v>L32</v>
       </c>
     </row>
-    <row r="24" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
-      <c r="B24" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="29"/>
-      <c r="D24" s="30" t="s">
+    <row r="24" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A24" s="39"/>
+      <c r="B24" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="41"/>
+      <c r="D24" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="32" t="s">
+      <c r="E24" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="F24" s="33"/>
+      <c r="F24" s="45"/>
       <c r="G24" s="18">
         <f>LaneData!S8</f>
         <v>0</v>
@@ -4478,18 +4451,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="27"/>
-      <c r="B25" s="34">
+    <row r="25" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A25" s="39"/>
+      <c r="B25" s="46">
         <f>LaneData!A18</f>
-        <v>55</v>
-      </c>
-      <c r="C25" s="35"/>
-      <c r="D25" s="31"/>
+        <v>0</v>
+      </c>
+      <c r="C25" s="47"/>
+      <c r="D25" s="43"/>
       <c r="E25" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="F25" s="48"/>
+      <c r="F25" s="38"/>
       <c r="G25" s="18">
         <f>LaneData!S9</f>
         <v>0</v>
@@ -4555,17 +4528,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="27"/>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="30" t="s">
+    <row r="26" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A26" s="39"/>
+      <c r="B26" s="48"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="E26" s="42" t="s">
-        <v>115</v>
-      </c>
-      <c r="F26" s="33"/>
+      <c r="E26" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="F26" s="45"/>
       <c r="G26" s="18">
         <f>LaneData!S10</f>
         <v>0</v>
@@ -4631,17 +4604,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="27"/>
-      <c r="B27" s="43" t="s">
+    <row r="27" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A27" s="39"/>
+      <c r="B27" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="44"/>
+      <c r="C27" s="56"/>
       <c r="D27" s="60"/>
-      <c r="E27" s="45" t="s">
-        <v>116</v>
-      </c>
-      <c r="F27" s="46"/>
+      <c r="E27" s="57" t="s">
+        <v>107</v>
+      </c>
+      <c r="F27" s="58"/>
       <c r="G27" s="18">
         <f>LaneData!S11</f>
         <v>0</v>
@@ -4707,15 +4680,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" ht="40.5" customHeight="1">
       <c r="A28" s="10"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="47" t="s">
-        <v>117</v>
-      </c>
-      <c r="F28" s="48"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="F28" s="38"/>
       <c r="G28" s="18">
         <f>LaneData!S12</f>
         <v>0</v>
@@ -4781,7 +4754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:22" s="11" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" s="11" customFormat="1" ht="10.5" customHeight="1">
       <c r="A29" s="9"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -4805,12 +4778,12 @@
       <c r="U29" s="15"/>
       <c r="V29" s="15"/>
     </row>
-    <row r="30" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:22" ht="21" customHeight="1">
       <c r="A30" s="16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="1:22" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" ht="26.25" customHeight="1">
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
@@ -4834,7 +4807,7 @@
       <c r="U31" s="13"/>
       <c r="V31" s="13"/>
     </row>
-    <row r="32" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" ht="40.5" customHeight="1">
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
       <c r="C32" s="13"/>
@@ -4858,7 +4831,7 @@
       <c r="U32" s="13"/>
       <c r="V32" s="13"/>
     </row>
-    <row r="33" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" ht="40.5" customHeight="1">
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
       <c r="C33" s="13"/>
@@ -4882,11 +4855,41 @@
       <c r="U33" s="13"/>
       <c r="V33" s="13"/>
     </row>
-    <row r="34" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" ht="15.75" customHeight="1">
       <c r="A34" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="43">
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="L3:Q3"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="B11:C12"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="B18:C19"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="D23:F23"/>
     <mergeCell ref="E28:F28"/>
@@ -4900,36 +4903,6 @@
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="E27:F27"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="B18:C19"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="B11:C12"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="L3:Q3"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:F9"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0.5" header="0" footer="0"/>
@@ -4952,7 +4925,7 @@
       <selection activeCell="E26" sqref="E26:F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
@@ -4962,55 +4935,55 @@
     <col min="7" max="22" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:22" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C3" s="51" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
+    <row r="3" spans="1:22" s="1" customFormat="1" ht="27" customHeight="1">
+      <c r="C3" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
       <c r="F3" s="3" t="str">
         <f>LaneData!B5</f>
         <v>300</v>
       </c>
-      <c r="H3" s="52" t="s">
+      <c r="H3" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="50" t="str">
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="28" t="str">
         <f>LaneData!B3</f>
         <v>USBC_Data_1-4_O</v>
       </c>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50"/>
-      <c r="Q3" s="50"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
+      <c r="Q3" s="28"/>
       <c r="S3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="T3" s="49" t="str">
+      <c r="T3" s="27" t="str">
         <f>LaneData!B4</f>
         <v>2/2/2012</v>
       </c>
-      <c r="U3" s="49"/>
-    </row>
-    <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="U3" s="27"/>
+    </row>
+    <row r="4" spans="1:22" ht="15" customHeight="1"/>
+    <row r="5" spans="1:22" ht="18.75" customHeight="1">
       <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" ht="18.75" customHeight="1">
       <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" ht="18.75" customHeight="1">
       <c r="A7" s="4"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22">
       <c r="G8" s="5" t="s">
         <v>5</v>
       </c>
@@ -5060,17 +5033,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" ht="40.5" customHeight="1">
       <c r="A9" s="6"/>
-      <c r="B9" s="58" t="s">
+      <c r="B9" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="54"/>
-      <c r="D9" s="55" t="s">
+      <c r="C9" s="32"/>
+      <c r="D9" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
       <c r="G9" s="7" t="str">
         <f>LaneData!AI7</f>
         <v>L33</v>
@@ -5136,19 +5109,19 @@
         <v>L48</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
-      <c r="B10" s="28" t="s">
+    <row r="10" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A10" s="39"/>
+      <c r="B10" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="29"/>
-      <c r="D10" s="30" t="s">
+      <c r="C10" s="41"/>
+      <c r="D10" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="32" t="s">
+      <c r="E10" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="33"/>
+      <c r="F10" s="45"/>
       <c r="G10" s="18">
         <f>LaneData!AI8</f>
         <v>0</v>
@@ -5214,18 +5187,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
-      <c r="B11" s="34">
+    <row r="11" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A11" s="39"/>
+      <c r="B11" s="46">
         <f>LaneData!A8</f>
-        <v>15</v>
-      </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="31"/>
+        <v>0</v>
+      </c>
+      <c r="C11" s="47"/>
+      <c r="D11" s="43"/>
       <c r="E11" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="48"/>
+      <c r="F11" s="38"/>
       <c r="G11" s="18">
         <f>LaneData!AI9</f>
         <v>0</v>
@@ -5291,17 +5264,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="30" t="s">
+    <row r="12" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A12" s="39"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="42" t="s">
-        <v>115</v>
-      </c>
-      <c r="F12" s="33"/>
+      <c r="E12" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="F12" s="45"/>
       <c r="G12" s="18">
         <f>LaneData!AI10</f>
         <v>0</v>
@@ -5367,17 +5340,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
-      <c r="B13" s="43" t="s">
+    <row r="13" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A13" s="39"/>
+      <c r="B13" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="44"/>
+      <c r="C13" s="56"/>
       <c r="D13" s="60"/>
-      <c r="E13" s="45" t="s">
-        <v>116</v>
-      </c>
-      <c r="F13" s="46"/>
+      <c r="E13" s="57" t="s">
+        <v>107</v>
+      </c>
+      <c r="F13" s="58"/>
       <c r="G13" s="18">
         <f>LaneData!AI11</f>
         <v>0</v>
@@ -5443,15 +5416,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" ht="40.5" customHeight="1">
       <c r="A14" s="9"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="47" t="s">
-        <v>117</v>
-      </c>
-      <c r="F14" s="48"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="F14" s="38"/>
       <c r="G14" s="18">
         <f>LaneData!AI12</f>
         <v>0</v>
@@ -5517,7 +5490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22">
       <c r="A15" s="11"/>
       <c r="B15" s="12"/>
       <c r="G15" s="5" t="s">
@@ -5569,17 +5542,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" ht="40.5" customHeight="1">
       <c r="A16" s="6"/>
-      <c r="B16" s="56" t="s">
+      <c r="B16" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="57"/>
-      <c r="D16" s="55" t="s">
+      <c r="C16" s="35"/>
+      <c r="D16" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
       <c r="G16" s="7" t="str">
         <f>LaneData!AI7</f>
         <v>L33</v>
@@ -5645,19 +5618,19 @@
         <v>L48</v>
       </c>
     </row>
-    <row r="17" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
-      <c r="B17" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="29"/>
-      <c r="D17" s="30" t="s">
+    <row r="17" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A17" s="39"/>
+      <c r="B17" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="41"/>
+      <c r="D17" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="32" t="s">
+      <c r="E17" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="33"/>
+      <c r="F17" s="45"/>
       <c r="G17" s="18">
         <f>LaneData!AI8</f>
         <v>0</v>
@@ -5723,18 +5696,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
-      <c r="B18" s="34">
+    <row r="18" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A18" s="39"/>
+      <c r="B18" s="46">
         <f>LaneData!A13</f>
-        <v>30</v>
-      </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="31"/>
+        <v>0</v>
+      </c>
+      <c r="C18" s="47"/>
+      <c r="D18" s="43"/>
       <c r="E18" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="48"/>
+      <c r="F18" s="38"/>
       <c r="G18" s="18">
         <f>LaneData!AI9</f>
         <v>0</v>
@@ -5800,17 +5773,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="30" t="s">
+    <row r="19" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A19" s="39"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="42" t="s">
-        <v>115</v>
-      </c>
-      <c r="F19" s="33"/>
+      <c r="E19" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="F19" s="45"/>
       <c r="G19" s="18">
         <f>LaneData!AI10</f>
         <v>0</v>
@@ -5876,17 +5849,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
-      <c r="B20" s="43" t="s">
+    <row r="20" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A20" s="39"/>
+      <c r="B20" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="44"/>
+      <c r="C20" s="56"/>
       <c r="D20" s="60"/>
-      <c r="E20" s="45" t="s">
-        <v>116</v>
-      </c>
-      <c r="F20" s="46"/>
+      <c r="E20" s="57" t="s">
+        <v>107</v>
+      </c>
+      <c r="F20" s="58"/>
       <c r="G20" s="18">
         <f>LaneData!AI11</f>
         <v>0</v>
@@ -5952,15 +5925,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" ht="40.5" customHeight="1">
       <c r="A21" s="9"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="47" t="s">
-        <v>117</v>
-      </c>
-      <c r="F21" s="48"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="F21" s="38"/>
       <c r="G21" s="18">
         <f>LaneData!AI12</f>
         <v>0</v>
@@ -6026,7 +5999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22">
       <c r="A22" s="11"/>
       <c r="B22" s="13"/>
       <c r="G22" s="5" t="s">
@@ -6078,17 +6051,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" ht="40.5" customHeight="1">
       <c r="A23" s="6"/>
-      <c r="B23" s="53" t="s">
+      <c r="B23" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="54"/>
-      <c r="D23" s="55" t="s">
+      <c r="C23" s="32"/>
+      <c r="D23" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="55"/>
-      <c r="F23" s="55"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="33"/>
       <c r="G23" s="7" t="str">
         <f>LaneData!AI7</f>
         <v>L33</v>
@@ -6154,19 +6127,19 @@
         <v>L48</v>
       </c>
     </row>
-    <row r="24" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
-      <c r="B24" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="29"/>
-      <c r="D24" s="30" t="s">
+    <row r="24" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A24" s="39"/>
+      <c r="B24" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="41"/>
+      <c r="D24" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="32" t="s">
+      <c r="E24" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="F24" s="33"/>
+      <c r="F24" s="45"/>
       <c r="G24" s="18">
         <f>LaneData!AI8</f>
         <v>0</v>
@@ -6232,18 +6205,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="27"/>
-      <c r="B25" s="34">
+    <row r="25" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A25" s="39"/>
+      <c r="B25" s="46">
         <f>LaneData!A18</f>
-        <v>55</v>
-      </c>
-      <c r="C25" s="35"/>
-      <c r="D25" s="31"/>
+        <v>0</v>
+      </c>
+      <c r="C25" s="47"/>
+      <c r="D25" s="43"/>
       <c r="E25" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="F25" s="48"/>
+      <c r="F25" s="38"/>
       <c r="G25" s="18">
         <f>LaneData!AI9</f>
         <v>0</v>
@@ -6309,17 +6282,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="27"/>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="30" t="s">
+    <row r="26" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A26" s="39"/>
+      <c r="B26" s="48"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="E26" s="42" t="s">
-        <v>115</v>
-      </c>
-      <c r="F26" s="33"/>
+      <c r="E26" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="F26" s="45"/>
       <c r="G26" s="18">
         <f>LaneData!AI10</f>
         <v>0</v>
@@ -6385,17 +6358,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="27"/>
-      <c r="B27" s="43" t="s">
+    <row r="27" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A27" s="39"/>
+      <c r="B27" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="44"/>
+      <c r="C27" s="56"/>
       <c r="D27" s="60"/>
-      <c r="E27" s="45" t="s">
-        <v>116</v>
-      </c>
-      <c r="F27" s="46"/>
+      <c r="E27" s="57" t="s">
+        <v>107</v>
+      </c>
+      <c r="F27" s="58"/>
       <c r="G27" s="18">
         <f>LaneData!AI11</f>
         <v>0</v>
@@ -6461,15 +6434,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" ht="40.5" customHeight="1">
       <c r="A28" s="10"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="47" t="s">
-        <v>117</v>
-      </c>
-      <c r="F28" s="48"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="F28" s="38"/>
       <c r="G28" s="18">
         <f>LaneData!AI12</f>
         <v>0</v>
@@ -6535,7 +6508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:22" s="11" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" s="11" customFormat="1" ht="10.5" customHeight="1">
       <c r="A29" s="9"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -6559,12 +6532,12 @@
       <c r="U29" s="15"/>
       <c r="V29" s="15"/>
     </row>
-    <row r="30" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:22" ht="21" customHeight="1">
       <c r="A30" s="16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="1:22" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" ht="26.25" customHeight="1">
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
@@ -6588,7 +6561,7 @@
       <c r="U31" s="13"/>
       <c r="V31" s="13"/>
     </row>
-    <row r="32" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" ht="40.5" customHeight="1">
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
       <c r="C32" s="13"/>
@@ -6612,7 +6585,7 @@
       <c r="U32" s="13"/>
       <c r="V32" s="13"/>
     </row>
-    <row r="33" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" ht="40.5" customHeight="1">
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
       <c r="C33" s="13"/>
@@ -6636,11 +6609,41 @@
       <c r="U33" s="13"/>
       <c r="V33" s="13"/>
     </row>
-    <row r="34" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" ht="15.75" customHeight="1">
       <c r="A34" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="43">
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="L3:Q3"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="B11:C12"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="B18:C19"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="D23:F23"/>
     <mergeCell ref="E28:F28"/>
@@ -6654,36 +6657,6 @@
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="E27:F27"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="B18:C19"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="B11:C12"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="L3:Q3"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:F9"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0.5" header="0" footer="0"/>
@@ -6706,7 +6679,7 @@
       <selection activeCell="E26" sqref="E26:F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
@@ -6717,55 +6690,55 @@
     <col min="8" max="22" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:22" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C3" s="51" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
+    <row r="3" spans="1:22" s="1" customFormat="1" ht="27" customHeight="1">
+      <c r="C3" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
       <c r="F3" s="3" t="str">
         <f>LaneData!B5</f>
         <v>300</v>
       </c>
-      <c r="H3" s="52" t="s">
+      <c r="H3" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="50" t="str">
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="28" t="str">
         <f>LaneData!B3</f>
         <v>USBC_Data_1-4_O</v>
       </c>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50"/>
-      <c r="Q3" s="50"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
+      <c r="Q3" s="28"/>
       <c r="S3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="T3" s="49" t="str">
+      <c r="T3" s="27" t="str">
         <f>LaneData!B4</f>
         <v>2/2/2012</v>
       </c>
-      <c r="U3" s="49"/>
-    </row>
-    <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="U3" s="27"/>
+    </row>
+    <row r="4" spans="1:22" ht="15" customHeight="1"/>
+    <row r="5" spans="1:22" ht="18.75" customHeight="1">
       <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" ht="18.75" customHeight="1">
       <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" ht="18.75" customHeight="1">
       <c r="A7" s="4"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22">
       <c r="G8" s="5" t="s">
         <v>5</v>
       </c>
@@ -6815,17 +6788,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" ht="40.5" customHeight="1">
       <c r="A9" s="6"/>
-      <c r="B9" s="58" t="s">
+      <c r="B9" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="54"/>
-      <c r="D9" s="55" t="s">
+      <c r="C9" s="32"/>
+      <c r="D9" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
       <c r="G9" s="7" t="str">
         <f>LaneData!AY7</f>
         <v>L49</v>
@@ -6891,19 +6864,19 @@
         <v>L64</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
-      <c r="B10" s="28" t="s">
+    <row r="10" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A10" s="39"/>
+      <c r="B10" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="29"/>
-      <c r="D10" s="30" t="s">
+      <c r="C10" s="41"/>
+      <c r="D10" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="32" t="s">
+      <c r="E10" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="33"/>
+      <c r="F10" s="45"/>
       <c r="G10" s="18">
         <f>LaneData!AY8</f>
         <v>0</v>
@@ -6969,18 +6942,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
-      <c r="B11" s="34">
+    <row r="11" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A11" s="39"/>
+      <c r="B11" s="46">
         <f>LaneData!A8</f>
-        <v>15</v>
-      </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="31"/>
+        <v>0</v>
+      </c>
+      <c r="C11" s="47"/>
+      <c r="D11" s="43"/>
       <c r="E11" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="48"/>
+      <c r="F11" s="38"/>
       <c r="G11" s="18">
         <f>LaneData!AY9</f>
         <v>0</v>
@@ -7046,17 +7019,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="30" t="s">
+    <row r="12" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A12" s="39"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="42" t="s">
-        <v>115</v>
-      </c>
-      <c r="F12" s="33"/>
+      <c r="E12" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="F12" s="45"/>
       <c r="G12" s="18">
         <f>LaneData!AY10</f>
         <v>0</v>
@@ -7122,17 +7095,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
-      <c r="B13" s="43" t="s">
+    <row r="13" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A13" s="39"/>
+      <c r="B13" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="44"/>
+      <c r="C13" s="56"/>
       <c r="D13" s="60"/>
-      <c r="E13" s="45" t="s">
-        <v>116</v>
-      </c>
-      <c r="F13" s="46"/>
+      <c r="E13" s="57" t="s">
+        <v>107</v>
+      </c>
+      <c r="F13" s="58"/>
       <c r="G13" s="18">
         <f>LaneData!AY11</f>
         <v>0</v>
@@ -7198,15 +7171,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" ht="40.5" customHeight="1">
       <c r="A14" s="9"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="47" t="s">
-        <v>117</v>
-      </c>
-      <c r="F14" s="48"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="F14" s="38"/>
       <c r="G14" s="18">
         <f>LaneData!AY12</f>
         <v>0</v>
@@ -7272,7 +7245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22">
       <c r="A15" s="11"/>
       <c r="B15" s="12"/>
       <c r="G15" s="5" t="s">
@@ -7324,17 +7297,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" ht="40.5" customHeight="1">
       <c r="A16" s="6"/>
-      <c r="B16" s="56" t="s">
+      <c r="B16" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="57"/>
-      <c r="D16" s="55" t="s">
+      <c r="C16" s="35"/>
+      <c r="D16" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
       <c r="G16" s="7" t="str">
         <f>LaneData!AY7</f>
         <v>L49</v>
@@ -7400,19 +7373,19 @@
         <v>L64</v>
       </c>
     </row>
-    <row r="17" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
-      <c r="B17" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="29"/>
-      <c r="D17" s="30" t="s">
+    <row r="17" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A17" s="39"/>
+      <c r="B17" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="41"/>
+      <c r="D17" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="32" t="s">
+      <c r="E17" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="33"/>
+      <c r="F17" s="45"/>
       <c r="G17" s="18">
         <f>LaneData!AY8</f>
         <v>0</v>
@@ -7478,18 +7451,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
-      <c r="B18" s="34">
+    <row r="18" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A18" s="39"/>
+      <c r="B18" s="46">
         <f>LaneData!A13</f>
-        <v>30</v>
-      </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="31"/>
+        <v>0</v>
+      </c>
+      <c r="C18" s="47"/>
+      <c r="D18" s="43"/>
       <c r="E18" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="48"/>
+      <c r="F18" s="38"/>
       <c r="G18" s="18">
         <f>LaneData!AY9</f>
         <v>0</v>
@@ -7555,17 +7528,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="30" t="s">
+    <row r="19" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A19" s="39"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="42" t="s">
-        <v>115</v>
-      </c>
-      <c r="F19" s="33"/>
+      <c r="E19" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="F19" s="45"/>
       <c r="G19" s="18">
         <f>LaneData!AY10</f>
         <v>0</v>
@@ -7631,17 +7604,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
-      <c r="B20" s="43" t="s">
+    <row r="20" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A20" s="39"/>
+      <c r="B20" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="44"/>
+      <c r="C20" s="56"/>
       <c r="D20" s="60"/>
-      <c r="E20" s="45" t="s">
-        <v>116</v>
-      </c>
-      <c r="F20" s="46"/>
+      <c r="E20" s="57" t="s">
+        <v>107</v>
+      </c>
+      <c r="F20" s="58"/>
       <c r="G20" s="18">
         <f>LaneData!AY11</f>
         <v>0</v>
@@ -7707,15 +7680,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" ht="40.5" customHeight="1">
       <c r="A21" s="9"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="47" t="s">
-        <v>117</v>
-      </c>
-      <c r="F21" s="48"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="F21" s="38"/>
       <c r="G21" s="18">
         <f>LaneData!AY12</f>
         <v>0</v>
@@ -7781,7 +7754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22">
       <c r="A22" s="11"/>
       <c r="B22" s="13"/>
       <c r="G22" s="5" t="s">
@@ -7833,17 +7806,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" ht="40.5" customHeight="1">
       <c r="A23" s="6"/>
-      <c r="B23" s="53" t="s">
+      <c r="B23" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="54"/>
-      <c r="D23" s="55" t="s">
+      <c r="C23" s="32"/>
+      <c r="D23" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="55"/>
-      <c r="F23" s="55"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="33"/>
       <c r="G23" s="7" t="str">
         <f>LaneData!AY7</f>
         <v>L49</v>
@@ -7909,19 +7882,19 @@
         <v>L64</v>
       </c>
     </row>
-    <row r="24" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
-      <c r="B24" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="29"/>
-      <c r="D24" s="30" t="s">
+    <row r="24" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A24" s="39"/>
+      <c r="B24" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="41"/>
+      <c r="D24" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="32" t="s">
+      <c r="E24" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="F24" s="33"/>
+      <c r="F24" s="45"/>
       <c r="G24" s="18">
         <f>LaneData!AY8</f>
         <v>0</v>
@@ -7987,18 +7960,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="27"/>
-      <c r="B25" s="34">
+    <row r="25" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A25" s="39"/>
+      <c r="B25" s="46">
         <f>LaneData!A18</f>
-        <v>55</v>
-      </c>
-      <c r="C25" s="35"/>
-      <c r="D25" s="31"/>
+        <v>0</v>
+      </c>
+      <c r="C25" s="47"/>
+      <c r="D25" s="43"/>
       <c r="E25" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="F25" s="48"/>
+      <c r="F25" s="38"/>
       <c r="G25" s="18">
         <f>LaneData!AY9</f>
         <v>0</v>
@@ -8064,17 +8037,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="27"/>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="30" t="s">
+    <row r="26" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A26" s="39"/>
+      <c r="B26" s="48"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="E26" s="42" t="s">
-        <v>115</v>
-      </c>
-      <c r="F26" s="33"/>
+      <c r="E26" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="F26" s="45"/>
       <c r="G26" s="18">
         <f>LaneData!AY10</f>
         <v>0</v>
@@ -8140,17 +8113,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="27"/>
-      <c r="B27" s="43" t="s">
+    <row r="27" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A27" s="39"/>
+      <c r="B27" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="44"/>
+      <c r="C27" s="56"/>
       <c r="D27" s="60"/>
-      <c r="E27" s="45" t="s">
-        <v>116</v>
-      </c>
-      <c r="F27" s="46"/>
+      <c r="E27" s="57" t="s">
+        <v>107</v>
+      </c>
+      <c r="F27" s="58"/>
       <c r="G27" s="18">
         <f>LaneData!AY11</f>
         <v>0</v>
@@ -8216,15 +8189,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" ht="40.5" customHeight="1">
       <c r="A28" s="10"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="47" t="s">
-        <v>117</v>
-      </c>
-      <c r="F28" s="48"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="F28" s="38"/>
       <c r="G28" s="18">
         <f>LaneData!AY12</f>
         <v>0</v>
@@ -8290,7 +8263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:22" s="11" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" s="11" customFormat="1" ht="10.5" customHeight="1">
       <c r="A29" s="9"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -8314,12 +8287,12 @@
       <c r="U29" s="15"/>
       <c r="V29" s="15"/>
     </row>
-    <row r="30" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:22" ht="21" customHeight="1">
       <c r="A30" s="16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="1:22" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" ht="26.25" customHeight="1">
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
@@ -8343,7 +8316,7 @@
       <c r="U31" s="13"/>
       <c r="V31" s="13"/>
     </row>
-    <row r="32" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" ht="40.5" customHeight="1">
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
       <c r="C32" s="13"/>
@@ -8367,7 +8340,7 @@
       <c r="U32" s="13"/>
       <c r="V32" s="13"/>
     </row>
-    <row r="33" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" ht="40.5" customHeight="1">
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
       <c r="C33" s="13"/>
@@ -8391,11 +8364,41 @@
       <c r="U33" s="13"/>
       <c r="V33" s="13"/>
     </row>
-    <row r="34" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" ht="15.75" customHeight="1">
       <c r="A34" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="43">
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="L3:Q3"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="B11:C12"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="B18:C19"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="D23:F23"/>
     <mergeCell ref="E28:F28"/>
@@ -8409,36 +8412,6 @@
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="E27:F27"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="B18:C19"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="B11:C12"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="L3:Q3"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:F9"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0.5" header="0" footer="0"/>
@@ -8461,7 +8434,7 @@
       <selection activeCell="E26" sqref="E26:F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
@@ -8471,55 +8444,55 @@
     <col min="7" max="22" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:22" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C3" s="51" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
+    <row r="3" spans="1:22" s="1" customFormat="1" ht="27" customHeight="1">
+      <c r="C3" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
       <c r="F3" s="3" t="str">
         <f>LaneData!B5</f>
         <v>300</v>
       </c>
-      <c r="H3" s="52" t="s">
+      <c r="H3" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="50" t="str">
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="28" t="str">
         <f>LaneData!B3</f>
         <v>USBC_Data_1-4_O</v>
       </c>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50"/>
-      <c r="Q3" s="50"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
+      <c r="Q3" s="28"/>
       <c r="S3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="T3" s="49" t="str">
+      <c r="T3" s="27" t="str">
         <f>LaneData!B4</f>
         <v>2/2/2012</v>
       </c>
-      <c r="U3" s="49"/>
-    </row>
-    <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="U3" s="27"/>
+    </row>
+    <row r="4" spans="1:22" ht="15" customHeight="1"/>
+    <row r="5" spans="1:22" ht="18.75" customHeight="1">
       <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" ht="18.75" customHeight="1">
       <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" ht="18.75" customHeight="1">
       <c r="A7" s="4"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22">
       <c r="G8" s="5" t="s">
         <v>5</v>
       </c>
@@ -8569,17 +8542,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" ht="40.5" customHeight="1">
       <c r="A9" s="6"/>
-      <c r="B9" s="58" t="s">
+      <c r="B9" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="54"/>
-      <c r="D9" s="55" t="s">
+      <c r="C9" s="32"/>
+      <c r="D9" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="55"/>
-      <c r="F9" s="55"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
       <c r="G9" s="7" t="str">
         <f>LaneData!BO7</f>
         <v>L65</v>
@@ -8645,19 +8618,19 @@
         <v>L80</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
-      <c r="B10" s="28" t="s">
+    <row r="10" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A10" s="39"/>
+      <c r="B10" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="29"/>
-      <c r="D10" s="30" t="s">
+      <c r="C10" s="41"/>
+      <c r="D10" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="32" t="s">
+      <c r="E10" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="33"/>
+      <c r="F10" s="45"/>
       <c r="G10" s="18">
         <f>LaneData!BO8</f>
         <v>0</v>
@@ -8723,18 +8696,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
-      <c r="B11" s="34">
+    <row r="11" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A11" s="39"/>
+      <c r="B11" s="46">
         <f>LaneData!A8</f>
-        <v>15</v>
-      </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="31"/>
+        <v>0</v>
+      </c>
+      <c r="C11" s="47"/>
+      <c r="D11" s="43"/>
       <c r="E11" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="48"/>
+      <c r="F11" s="38"/>
       <c r="G11" s="18">
         <f>LaneData!BO9</f>
         <v>0</v>
@@ -8800,17 +8773,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="30" t="s">
+    <row r="12" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A12" s="39"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="42" t="s">
-        <v>115</v>
-      </c>
-      <c r="F12" s="33"/>
+      <c r="E12" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="F12" s="45"/>
       <c r="G12" s="18">
         <f>LaneData!BO10</f>
         <v>0</v>
@@ -8876,17 +8849,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
-      <c r="B13" s="43" t="s">
+    <row r="13" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A13" s="39"/>
+      <c r="B13" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="44"/>
+      <c r="C13" s="56"/>
       <c r="D13" s="60"/>
-      <c r="E13" s="45" t="s">
-        <v>116</v>
-      </c>
-      <c r="F13" s="46"/>
+      <c r="E13" s="57" t="s">
+        <v>107</v>
+      </c>
+      <c r="F13" s="58"/>
       <c r="G13" s="18">
         <f>LaneData!BO11</f>
         <v>0</v>
@@ -8952,15 +8925,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" ht="40.5" customHeight="1">
       <c r="A14" s="9"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="47" t="s">
-        <v>117</v>
-      </c>
-      <c r="F14" s="48"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="F14" s="38"/>
       <c r="G14" s="18">
         <f>LaneData!BO12</f>
         <v>0</v>
@@ -9026,7 +8999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22">
       <c r="A15" s="11"/>
       <c r="B15" s="12"/>
       <c r="G15" s="5" t="s">
@@ -9078,17 +9051,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" ht="40.5" customHeight="1">
       <c r="A16" s="6"/>
-      <c r="B16" s="56" t="s">
+      <c r="B16" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="57"/>
-      <c r="D16" s="55" t="s">
+      <c r="C16" s="35"/>
+      <c r="D16" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
       <c r="G16" s="7" t="str">
         <f>LaneData!BO7</f>
         <v>L65</v>
@@ -9154,19 +9127,19 @@
         <v>L80</v>
       </c>
     </row>
-    <row r="17" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
-      <c r="B17" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="29"/>
-      <c r="D17" s="30" t="s">
+    <row r="17" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A17" s="39"/>
+      <c r="B17" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="41"/>
+      <c r="D17" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="32" t="s">
+      <c r="E17" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="33"/>
+      <c r="F17" s="45"/>
       <c r="G17" s="18">
         <f>LaneData!BO8</f>
         <v>0</v>
@@ -9232,18 +9205,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
-      <c r="B18" s="34">
+    <row r="18" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A18" s="39"/>
+      <c r="B18" s="46">
         <f>LaneData!A13</f>
-        <v>30</v>
-      </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="31"/>
+        <v>0</v>
+      </c>
+      <c r="C18" s="47"/>
+      <c r="D18" s="43"/>
       <c r="E18" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="48"/>
+      <c r="F18" s="38"/>
       <c r="G18" s="18">
         <f>LaneData!BO9</f>
         <v>0</v>
@@ -9309,17 +9282,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="30" t="s">
+    <row r="19" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A19" s="39"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="42" t="s">
-        <v>115</v>
-      </c>
-      <c r="F19" s="33"/>
+      <c r="E19" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="F19" s="45"/>
       <c r="G19" s="18">
         <f>LaneData!BO10</f>
         <v>0</v>
@@ -9385,17 +9358,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
-      <c r="B20" s="43" t="s">
+    <row r="20" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A20" s="39"/>
+      <c r="B20" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="44"/>
+      <c r="C20" s="56"/>
       <c r="D20" s="60"/>
-      <c r="E20" s="45" t="s">
-        <v>116</v>
-      </c>
-      <c r="F20" s="46"/>
+      <c r="E20" s="57" t="s">
+        <v>107</v>
+      </c>
+      <c r="F20" s="58"/>
       <c r="G20" s="18">
         <f>LaneData!BO11</f>
         <v>0</v>
@@ -9461,15 +9434,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" ht="40.5" customHeight="1">
       <c r="A21" s="9"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="47" t="s">
-        <v>117</v>
-      </c>
-      <c r="F21" s="48"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="F21" s="38"/>
       <c r="G21" s="18">
         <f>LaneData!BO12</f>
         <v>0</v>
@@ -9535,7 +9508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22">
       <c r="A22" s="11"/>
       <c r="B22" s="13"/>
       <c r="G22" s="5" t="s">
@@ -9587,17 +9560,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" ht="40.5" customHeight="1">
       <c r="A23" s="6"/>
-      <c r="B23" s="53" t="s">
+      <c r="B23" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="54"/>
-      <c r="D23" s="55" t="s">
+      <c r="C23" s="32"/>
+      <c r="D23" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="55"/>
-      <c r="F23" s="55"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="33"/>
       <c r="G23" s="7" t="str">
         <f>LaneData!BO7</f>
         <v>L65</v>
@@ -9663,19 +9636,19 @@
         <v>L80</v>
       </c>
     </row>
-    <row r="24" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
-      <c r="B24" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="29"/>
-      <c r="D24" s="30" t="s">
+    <row r="24" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A24" s="39"/>
+      <c r="B24" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="41"/>
+      <c r="D24" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="32" t="s">
+      <c r="E24" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="F24" s="33"/>
+      <c r="F24" s="45"/>
       <c r="G24" s="18">
         <f>LaneData!BO8</f>
         <v>0</v>
@@ -9741,18 +9714,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="27"/>
-      <c r="B25" s="34">
+    <row r="25" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A25" s="39"/>
+      <c r="B25" s="46">
         <f>LaneData!A18</f>
-        <v>55</v>
-      </c>
-      <c r="C25" s="35"/>
-      <c r="D25" s="31"/>
+        <v>0</v>
+      </c>
+      <c r="C25" s="47"/>
+      <c r="D25" s="43"/>
       <c r="E25" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="F25" s="48"/>
+      <c r="F25" s="38"/>
       <c r="G25" s="18">
         <f>LaneData!BO9</f>
         <v>0</v>
@@ -9818,17 +9791,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="27"/>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="30" t="s">
+    <row r="26" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A26" s="39"/>
+      <c r="B26" s="48"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="E26" s="42" t="s">
-        <v>115</v>
-      </c>
-      <c r="F26" s="33"/>
+      <c r="E26" s="54" t="s">
+        <v>106</v>
+      </c>
+      <c r="F26" s="45"/>
       <c r="G26" s="18">
         <f>LaneData!BO10</f>
         <v>0</v>
@@ -9894,17 +9867,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="27"/>
-      <c r="B27" s="43" t="s">
+    <row r="27" spans="1:22" ht="40.5" customHeight="1">
+      <c r="A27" s="39"/>
+      <c r="B27" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="44"/>
+      <c r="C27" s="56"/>
       <c r="D27" s="60"/>
-      <c r="E27" s="45" t="s">
-        <v>116</v>
-      </c>
-      <c r="F27" s="46"/>
+      <c r="E27" s="57" t="s">
+        <v>107</v>
+      </c>
+      <c r="F27" s="58"/>
       <c r="G27" s="18">
         <f>LaneData!BO11</f>
         <v>0</v>
@@ -9970,15 +9943,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" ht="40.5" customHeight="1">
       <c r="A28" s="10"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="47" t="s">
-        <v>117</v>
-      </c>
-      <c r="F28" s="48"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="F28" s="38"/>
       <c r="G28" s="18">
         <f>LaneData!BO12</f>
         <v>0</v>
@@ -10044,7 +10017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:22" s="11" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" s="11" customFormat="1" ht="10.5" customHeight="1">
       <c r="A29" s="9"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -10068,12 +10041,12 @@
       <c r="U29" s="15"/>
       <c r="V29" s="15"/>
     </row>
-    <row r="30" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:22" ht="21" customHeight="1">
       <c r="A30" s="16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="1:22" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" ht="26.25" customHeight="1">
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
@@ -10097,7 +10070,7 @@
       <c r="U31" s="13"/>
       <c r="V31" s="13"/>
     </row>
-    <row r="32" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" ht="40.5" customHeight="1">
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
       <c r="C32" s="13"/>
@@ -10121,7 +10094,7 @@
       <c r="U32" s="13"/>
       <c r="V32" s="13"/>
     </row>
-    <row r="33" spans="1:22" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" ht="40.5" customHeight="1">
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
       <c r="C33" s="13"/>
@@ -10145,11 +10118,41 @@
       <c r="U33" s="13"/>
       <c r="V33" s="13"/>
     </row>
-    <row r="34" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" ht="15.75" customHeight="1">
       <c r="A34" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="43">
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="L3:Q3"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="B11:C12"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="B18:C19"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="D23:F23"/>
     <mergeCell ref="E28:F28"/>
@@ -10163,36 +10166,6 @@
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="E27:F27"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="B18:C19"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="B11:C12"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="L3:Q3"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:F9"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0.5" header="0" footer="0"/>
@@ -10209,21 +10182,21 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="LaneData"/>
-  <dimension ref="A1:CX22"/>
+  <dimension ref="A1:CX7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="CE7" sqref="CE7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="2" width="16.7109375" style="19" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:102" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:102" ht="16.5" customHeight="1">
       <c r="A1" s="61" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B1" s="61"/>
       <c r="C1" s="61"/>
@@ -10236,41 +10209,41 @@
       <c r="J1" s="20"/>
       <c r="K1" s="20"/>
     </row>
-    <row r="2" spans="1:102" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:102" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:102" ht="13.5" customHeight="1"/>
+    <row r="3" spans="1:102" s="21" customFormat="1">
       <c r="A3" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="62" t="s">
         <v>99</v>
-      </c>
-      <c r="B3" s="62" t="s">
-        <v>100</v>
       </c>
       <c r="C3" s="62"/>
       <c r="D3" s="62"/>
       <c r="E3" s="62"/>
     </row>
-    <row r="4" spans="1:102" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:102" s="21" customFormat="1">
       <c r="A4" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="B4" s="23" t="s">
+    </row>
+    <row r="5" spans="1:102" s="21" customFormat="1">
+      <c r="A5" s="22" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="5" spans="1:102" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="22" t="s">
+      <c r="B5" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="B5" s="24" t="s">
+    </row>
+    <row r="6" spans="1:102" s="22" customFormat="1"/>
+    <row r="7" spans="1:102">
+      <c r="A7" s="25" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="6" spans="1:102" s="22" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:102" x14ac:dyDescent="0.2">
-      <c r="A7" s="25" t="s">
+      <c r="B7" s="19" t="s">
         <v>105</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>106</v>
       </c>
       <c r="C7" s="26" t="s">
         <v>8</v>
@@ -10321,196 +10294,196 @@
         <v>23</v>
       </c>
       <c r="S7" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="T7" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="T7" s="26" t="s">
+      <c r="U7" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="U7" s="26" t="s">
+      <c r="V7" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="V7" s="26" t="s">
+      <c r="W7" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="W7" s="26" t="s">
+      <c r="X7" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="X7" s="26" t="s">
+      <c r="Y7" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="Y7" s="26" t="s">
+      <c r="Z7" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="Z7" s="26" t="s">
+      <c r="AA7" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="AA7" s="26" t="s">
+      <c r="AB7" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="AB7" s="26" t="s">
+      <c r="AC7" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AC7" s="26" t="s">
+      <c r="AD7" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="AD7" s="26" t="s">
+      <c r="AE7" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="AE7" s="26" t="s">
+      <c r="AF7" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="AF7" s="26" t="s">
+      <c r="AG7" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="AG7" s="26" t="s">
+      <c r="AH7" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="AH7" s="26" t="s">
+      <c r="AI7" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="AI7" s="26" t="s">
+      <c r="AJ7" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="AJ7" s="26" t="s">
+      <c r="AK7" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="AK7" s="26" t="s">
+      <c r="AL7" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="AL7" s="26" t="s">
+      <c r="AM7" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="AM7" s="26" t="s">
+      <c r="AN7" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="AN7" s="26" t="s">
+      <c r="AO7" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="AO7" s="26" t="s">
+      <c r="AP7" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="AP7" s="26" t="s">
+      <c r="AQ7" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="AQ7" s="26" t="s">
+      <c r="AR7" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="AR7" s="26" t="s">
+      <c r="AS7" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="AS7" s="26" t="s">
+      <c r="AT7" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="AT7" s="26" t="s">
+      <c r="AU7" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="AU7" s="26" t="s">
+      <c r="AV7" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="AV7" s="26" t="s">
+      <c r="AW7" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="AW7" s="26" t="s">
+      <c r="AX7" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="AX7" s="26" t="s">
+      <c r="AY7" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="AY7" s="26" t="s">
+      <c r="AZ7" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="AZ7" s="26" t="s">
+      <c r="BA7" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="BA7" s="26" t="s">
+      <c r="BB7" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="BB7" s="26" t="s">
+      <c r="BC7" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="BC7" s="26" t="s">
+      <c r="BD7" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="BD7" s="26" t="s">
+      <c r="BE7" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="BE7" s="26" t="s">
+      <c r="BF7" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="BF7" s="26" t="s">
+      <c r="BG7" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="BG7" s="26" t="s">
+      <c r="BH7" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="BH7" s="26" t="s">
+      <c r="BI7" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="BI7" s="26" t="s">
+      <c r="BJ7" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="BJ7" s="26" t="s">
+      <c r="BK7" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="BK7" s="26" t="s">
+      <c r="BL7" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="BL7" s="26" t="s">
+      <c r="BM7" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="BM7" s="26" t="s">
+      <c r="BN7" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="BN7" s="26" t="s">
+      <c r="BO7" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="BO7" s="26" t="s">
+      <c r="BP7" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="BP7" s="26" t="s">
+      <c r="BQ7" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="BQ7" s="26" t="s">
+      <c r="BR7" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="BR7" s="26" t="s">
+      <c r="BS7" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="BS7" s="26" t="s">
+      <c r="BT7" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="BT7" s="26" t="s">
+      <c r="BU7" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="BU7" s="26" t="s">
+      <c r="BV7" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="BV7" s="26" t="s">
+      <c r="BW7" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="BW7" s="26" t="s">
+      <c r="BX7" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="BX7" s="26" t="s">
+      <c r="BY7" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="BY7" s="26" t="s">
+      <c r="BZ7" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="BZ7" s="26" t="s">
+      <c r="CA7" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="CA7" s="26" t="s">
+      <c r="CB7" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="CB7" s="26" t="s">
+      <c r="CC7" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="CC7" s="26" t="s">
+      <c r="CD7" s="26" t="s">
         <v>96</v>
-      </c>
-      <c r="CD7" s="26" t="s">
-        <v>97</v>
       </c>
       <c r="CE7" s="26"/>
       <c r="CF7" s="26"/>
@@ -10533,351 +10506,6 @@
       <c r="CW7" s="26"/>
       <c r="CX7" s="26"/>
     </row>
-    <row r="8" spans="1:102" x14ac:dyDescent="0.2">
-      <c r="A8" s="19">
-        <v>15</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="C8" s="19">
-        <v>-11</v>
-      </c>
-      <c r="D8" s="19">
-        <v>-10</v>
-      </c>
-      <c r="E8" s="19">
-        <v>-12</v>
-      </c>
-      <c r="F8" s="19">
-        <v>-11</v>
-      </c>
-      <c r="G8" s="19">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:102" x14ac:dyDescent="0.2">
-      <c r="A9" s="19">
-        <v>15</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="C9" s="19">
-        <v>-56</v>
-      </c>
-      <c r="D9" s="19">
-        <v>-54</v>
-      </c>
-      <c r="E9" s="19">
-        <v>-57</v>
-      </c>
-      <c r="F9" s="19">
-        <v>-51</v>
-      </c>
-      <c r="G9" s="19">
-        <v>-55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:102" x14ac:dyDescent="0.2">
-      <c r="A10" s="19">
-        <v>15</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="C10" s="19">
-        <v>-7</v>
-      </c>
-      <c r="D10" s="19">
-        <v>-7</v>
-      </c>
-      <c r="E10" s="19">
-        <v>-7</v>
-      </c>
-      <c r="F10" s="19">
-        <v>-7</v>
-      </c>
-      <c r="G10" s="19">
-        <v>-7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:102" x14ac:dyDescent="0.2">
-      <c r="A11" s="19">
-        <v>15</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="19">
-        <v>-18</v>
-      </c>
-      <c r="D11" s="19">
-        <v>-18</v>
-      </c>
-      <c r="E11" s="19">
-        <v>-18</v>
-      </c>
-      <c r="F11" s="19">
-        <v>-18</v>
-      </c>
-      <c r="G11" s="19">
-        <v>-18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:102" x14ac:dyDescent="0.2">
-      <c r="A12" s="19">
-        <v>15</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="C12" s="19">
-        <v>-15</v>
-      </c>
-      <c r="D12" s="19">
-        <v>-15</v>
-      </c>
-      <c r="E12" s="19">
-        <v>-15</v>
-      </c>
-      <c r="F12" s="19">
-        <v>-15</v>
-      </c>
-      <c r="G12" s="19">
-        <v>-15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:102" x14ac:dyDescent="0.2">
-      <c r="A13" s="19">
-        <v>30</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="C13" s="19">
-        <v>-1</v>
-      </c>
-      <c r="D13" s="19">
-        <v>-3</v>
-      </c>
-      <c r="E13" s="19">
-        <v>-2</v>
-      </c>
-      <c r="F13" s="19">
-        <v>-3</v>
-      </c>
-      <c r="G13" s="19">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:102" x14ac:dyDescent="0.2">
-      <c r="A14" s="19">
-        <v>30</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="C14" s="19">
-        <v>-166</v>
-      </c>
-      <c r="D14" s="19">
-        <v>-171</v>
-      </c>
-      <c r="E14" s="19">
-        <v>-169</v>
-      </c>
-      <c r="F14" s="19">
-        <v>-172</v>
-      </c>
-      <c r="G14" s="19">
-        <v>-167</v>
-      </c>
-    </row>
-    <row r="15" spans="1:102" x14ac:dyDescent="0.2">
-      <c r="A15" s="19">
-        <v>30</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="C15" s="19">
-        <v>0</v>
-      </c>
-      <c r="D15" s="19">
-        <v>0</v>
-      </c>
-      <c r="E15" s="19">
-        <v>0</v>
-      </c>
-      <c r="F15" s="19">
-        <v>0</v>
-      </c>
-      <c r="G15" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:102" x14ac:dyDescent="0.2">
-      <c r="A16" s="19">
-        <v>30</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="19">
-        <v>3</v>
-      </c>
-      <c r="D16" s="19">
-        <v>3</v>
-      </c>
-      <c r="E16" s="19">
-        <v>3</v>
-      </c>
-      <c r="F16" s="19">
-        <v>3</v>
-      </c>
-      <c r="G16" s="19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="19">
-        <v>30</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="C17" s="19">
-        <v>4</v>
-      </c>
-      <c r="D17" s="19">
-        <v>4</v>
-      </c>
-      <c r="E17" s="19">
-        <v>4</v>
-      </c>
-      <c r="F17" s="19">
-        <v>4</v>
-      </c>
-      <c r="G17" s="19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="19">
-        <v>55</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="C18" s="19">
-        <v>-15</v>
-      </c>
-      <c r="D18" s="19">
-        <v>-9</v>
-      </c>
-      <c r="E18" s="19">
-        <v>-10</v>
-      </c>
-      <c r="F18" s="19">
-        <v>-8</v>
-      </c>
-      <c r="G18" s="19">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="19">
-        <v>55</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="C19" s="19">
-        <v>-139</v>
-      </c>
-      <c r="D19" s="19">
-        <v>-141</v>
-      </c>
-      <c r="E19" s="19">
-        <v>-144</v>
-      </c>
-      <c r="F19" s="19">
-        <v>-145</v>
-      </c>
-      <c r="G19" s="19">
-        <v>-138</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="19">
-        <v>55</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="C20" s="19">
-        <v>2</v>
-      </c>
-      <c r="D20" s="19">
-        <v>2</v>
-      </c>
-      <c r="E20" s="19">
-        <v>2</v>
-      </c>
-      <c r="F20" s="19">
-        <v>2</v>
-      </c>
-      <c r="G20" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="19">
-        <v>55</v>
-      </c>
-      <c r="B21" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="19">
-        <v>-5</v>
-      </c>
-      <c r="D21" s="19">
-        <v>-5</v>
-      </c>
-      <c r="E21" s="19">
-        <v>-5</v>
-      </c>
-      <c r="F21" s="19">
-        <v>-5</v>
-      </c>
-      <c r="G21" s="19">
-        <v>-5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="19">
-        <v>55</v>
-      </c>
-      <c r="B22" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="C22" s="19">
-        <v>2</v>
-      </c>
-      <c r="D22" s="19">
-        <v>2</v>
-      </c>
-      <c r="E22" s="19">
-        <v>2</v>
-      </c>
-      <c r="F22" s="19">
-        <v>2</v>
-      </c>
-      <c r="G22" s="19">
-        <v>2</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:E1"/>

</xml_diff>